<commit_message>
junit for bank,customer and atm added
</commit_message>
<xml_diff>
--- a/checKlist.xlsx
+++ b/checKlist.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
   <si>
     <t>Logger</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Code coverage</t>
+  </si>
+  <si>
+    <t>Deno</t>
   </si>
 </sst>
 </file>
@@ -400,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F11"/>
+  <dimension ref="A2:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,12 +416,12 @@
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -434,8 +437,11 @@
       <c r="F3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -455,7 +461,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -475,7 +481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -495,7 +501,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -515,17 +521,26 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -535,8 +550,17 @@
       <c r="C10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
atm denomination functionality added
</commit_message>
<xml_diff>
--- a/checKlist.xlsx
+++ b/checKlist.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
   <si>
     <t>Logger</t>
   </si>
@@ -62,13 +63,34 @@
   </si>
   <si>
     <t>Deno</t>
+  </si>
+  <si>
+    <t>TASK</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>validation of noOFDenomination</t>
+  </si>
+  <si>
+    <t>Reading message from property file</t>
+  </si>
+  <si>
+    <t>Service 2 service call</t>
+  </si>
+  <si>
+    <t>Exception Handling</t>
+  </si>
+  <si>
+    <t>Code Commenting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,7 +181,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -191,10 +213,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -226,7 +247,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -402,26 +422,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -441,7 +461,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -461,7 +481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -481,7 +501,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -501,7 +521,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -521,12 +541,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -540,7 +560,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -560,7 +580,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -578,6 +598,62 @@
       </c>
       <c r="F11" t="s">
         <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="101.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
freashly started new application
</commit_message>
<xml_diff>
--- a/checKlist.xlsx
+++ b/checKlist.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="19">
   <si>
     <t>Logger</t>
   </si>
@@ -72,44 +71,14 @@
     <t>STATUS</t>
   </si>
   <si>
-    <t>validation of noOFDenomination</t>
-  </si>
-  <si>
-    <t>Reading message from property file</t>
-  </si>
-  <si>
-    <t>Service 2 service call</t>
-  </si>
-  <si>
-    <t>Exception Handling</t>
-  </si>
-  <si>
-    <t>Code Commenting</t>
-  </si>
-  <si>
-    <t>Banking System  microService1</t>
-  </si>
-  <si>
-    <t>Bank</t>
-  </si>
-  <si>
-    <t>customer</t>
-  </si>
-  <si>
-    <t>account</t>
-  </si>
-  <si>
-    <t>transaction</t>
-  </si>
-  <si>
-    <t>denomination</t>
+    <t>not throwing my exception throwing null pointer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,7 +169,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -232,10 +201,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -267,7 +235,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -443,26 +410,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -482,7 +449,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -502,7 +469,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -522,7 +489,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -542,7 +509,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -562,12 +529,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -581,7 +548,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -601,7 +568,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -627,19 +594,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="101.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -647,83 +614,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>